<commit_message>
agreagdno eventos a vista de primera limpia
</commit_message>
<xml_diff>
--- a/SCADA/RemoteRuntime/tagsDeAplicacion.xlsx
+++ b/SCADA/RemoteRuntime/tagsDeAplicacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="15255" windowHeight="8190" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="23655" windowHeight="13035"/>
   </bookViews>
   <sheets>
     <sheet name="Registered Tag List" sheetId="9" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="123">
   <si>
     <t>Network Info</t>
   </si>
@@ -84,64 +84,283 @@
     <t>L21_MODO</t>
   </si>
   <si>
+    <t>modo actual de la linea 21</t>
+  </si>
+  <si>
     <t>L21_MODO_AUTO</t>
   </si>
   <si>
+    <t>valor del modo automatico de la linea 21</t>
+  </si>
+  <si>
     <t>L21_MODO_MANUAL</t>
   </si>
   <si>
+    <t>valor del modo manual de la linea 21</t>
+  </si>
+  <si>
     <t>L21_MODO_RESET</t>
   </si>
   <si>
+    <t>valor del modo reset de la linea 21</t>
+  </si>
+  <si>
     <t>L21_MODO_INICIO</t>
   </si>
   <si>
+    <t>valor del modo inicio de la linea 21</t>
+  </si>
+  <si>
     <t>L21_MODO_TRANS_INICIO_RESET</t>
   </si>
   <si>
+    <t>valor del modo transicion inicio-reset de la linea 21</t>
+  </si>
+  <si>
     <t>L21_MODO_TRANS_RESET_INICIO</t>
   </si>
   <si>
+    <t>valor del modo transicion reset-incio de la linea 21</t>
+  </si>
+  <si>
     <t>L21_MODO_TRANS_RESET_AUTO</t>
   </si>
   <si>
+    <t>valor del modo transicion reset-auto de la linea 21</t>
+  </si>
+  <si>
     <t>L21_MODO_TRANS_AUTO_RESET</t>
   </si>
   <si>
+    <t>valor del modo transicion auto-reset de la linea 21</t>
+  </si>
+  <si>
     <t>L21_MODO_TRANS_RESET_MANUAL</t>
   </si>
   <si>
+    <t>valor del modo transicion reset-manual de la linea 21</t>
+  </si>
+  <si>
     <t>L21_MODO_TRANS_MANUAL_RESET</t>
   </si>
   <si>
+    <t>valor del modo transicion manual-reset de la linea 21</t>
+  </si>
+  <si>
     <t>L21_SILO_21_MIN</t>
   </si>
   <si>
     <t>Usigned int32</t>
   </si>
   <si>
+    <t>minimo valor de trigo en l silo 21</t>
+  </si>
+  <si>
     <t>L21_SILO_21_MAX</t>
   </si>
   <si>
+    <t>maximo valor de trigo en el silo 21</t>
+  </si>
+  <si>
     <t>L21_SILO_22_MIN</t>
   </si>
   <si>
+    <t>minimo valor de trgo en el silo 22</t>
+  </si>
+  <si>
     <t>L21_SILO_22_MAX</t>
   </si>
   <si>
+    <t>maximo valor de trigo en el silo 22</t>
+  </si>
+  <si>
     <t>L21_SILO_34_MIN</t>
   </si>
   <si>
+    <t>minimo valor de trigo en el silo 34</t>
+  </si>
+  <si>
     <t>L21_SILO_34_MAX</t>
   </si>
   <si>
-    <t>L21_CANTIDAD</t>
-  </si>
-  <si>
-    <t>l21TxtCantidad</t>
-  </si>
-  <si>
-    <t>l21NuevaVar</t>
+    <t>maximo vaor de trigo en el silo 34</t>
+  </si>
+  <si>
+    <t>L21_CANTIDAD_DESTINO</t>
+  </si>
+  <si>
+    <t>valor a tranferir en el silo de destino de la linea 21</t>
+  </si>
+  <si>
+    <t>L21_TIEMPO_VACIADO</t>
+  </si>
+  <si>
+    <t>tiempo de vaciado para la linea 21</t>
+  </si>
+  <si>
+    <t>L21_TIEMPO_BYPASS</t>
+  </si>
+  <si>
+    <t>timepo de bypass para la linea 21</t>
+  </si>
+  <si>
+    <t>L21_PUESTA_EN_MARCHA_COMPLEATA</t>
+  </si>
+  <si>
+    <t>flag de puesta en marcha linea 21 completa</t>
+  </si>
+  <si>
+    <t>l21TxtTiempoVaciado</t>
+  </si>
+  <si>
+    <t>valor textbox tiempo de vaciado en puesta en marcha linea 21</t>
+  </si>
+  <si>
+    <t>l21TxtTiempoByPass</t>
+  </si>
+  <si>
+    <t>valor textbox tiempo de bypass en puesta en marcha linea 21</t>
+  </si>
+  <si>
+    <t>L21_MIN_TIEMPO_VACIADO</t>
+  </si>
+  <si>
+    <t>minimo tiempo de vaciado/limpieaza para la linea 21</t>
+  </si>
+  <si>
+    <t>L21_MIN_TIEMPO_BYPASS</t>
+  </si>
+  <si>
+    <t>minimo tiempo de bypass para la linea 21</t>
+  </si>
+  <si>
+    <t>l21FrmPuestaEnMarchaEvent</t>
+  </si>
+  <si>
+    <t>variable para enviar señales al controlador de l21PuestaEnMarch</t>
+  </si>
+  <si>
+    <t>l21FrmPrimeraLineaEvent</t>
+  </si>
+  <si>
+    <t>almacena el evento a ejecutar en l21PrimeraLimpia</t>
+  </si>
+  <si>
+    <t>l21BtnPuestaEnMarchaEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de puesta en marcha de la L21</t>
+  </si>
+  <si>
+    <t>l21BtnResetEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de RESET en L21</t>
+  </si>
+  <si>
+    <t>l21BtnManualEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de MANUAL en L21</t>
+  </si>
+  <si>
+    <t>l21BtnAutomaticoEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de AUTOMATICO en L21</t>
+  </si>
+  <si>
+    <t>l21BtnInicioEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de INICION en L21</t>
+  </si>
+  <si>
+    <t>l21BtnTerminarEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de TERMINAR en L21</t>
+  </si>
+  <si>
+    <t>l21BtnParadaEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de PARADA en L21</t>
+  </si>
+  <si>
+    <t>l21BtnParadaInmediataEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de PARADA INMEDIATA  en L21</t>
+  </si>
+  <si>
+    <t>l21BtnContinuarEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de CONTINUAR en L21</t>
+  </si>
+  <si>
+    <t>l21BtnProximoSiloEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de PROXIMO SILO en L21</t>
+  </si>
+  <si>
+    <t>l21BtnActivarBypassEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de ACTIVAR BYPASS en L21</t>
+  </si>
+  <si>
+    <t>l21BtnDesactivarBypassEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de DESACTIVAR BYPASS en L21</t>
+  </si>
+  <si>
+    <t>l21CmbxOrigenEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el combobox de Origen en L21</t>
+  </si>
+  <si>
+    <t>l21CmbxOrigenValue</t>
+  </si>
+  <si>
+    <t>valor seleccionado en combobox de Origen en L21</t>
+  </si>
+  <si>
+    <t>l21CmbxDestinoEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el combobox de Destino en L21</t>
+  </si>
+  <si>
+    <t>l21CmbxDestinoValue</t>
+  </si>
+  <si>
+    <t>valor seleccionado en combobox de Destino en L21</t>
+  </si>
+  <si>
+    <t>l21BtnSalvarOrigenDestinoEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de SALVAR en L21</t>
+  </si>
+  <si>
+    <t>l21BtnCancelarOrigenDestinoEnabled</t>
+  </si>
+  <si>
+    <t>l21TxtCantidadOrigenDestino</t>
+  </si>
+  <si>
+    <t>valor del textbox Cantidad en L21</t>
+  </si>
+  <si>
+    <t>l21TxtCantidadOrgDesEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva textbox Cantidad en L21</t>
   </si>
   <si>
     <t>Server Name</t>
@@ -503,15 +722,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -675,13 +894,16 @@
       <c r="E9" t="s">
         <v>11</v>
       </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -692,13 +914,16 @@
       <c r="E10" t="s">
         <v>11</v>
       </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -708,6 +933,9 @@
       </c>
       <c r="E11" t="s">
         <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -715,7 +943,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -726,13 +954,16 @@
       <c r="E12" t="s">
         <v>11</v>
       </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -742,6 +973,9 @@
       </c>
       <c r="E13" t="s">
         <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -749,7 +983,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -760,13 +994,16 @@
       <c r="E14" t="s">
         <v>11</v>
       </c>
+      <c r="H14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -777,13 +1014,16 @@
       <c r="E15" t="s">
         <v>11</v>
       </c>
+      <c r="H15" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -794,13 +1034,16 @@
       <c r="E16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="H16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -811,13 +1054,16 @@
       <c r="E17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="H17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -828,13 +1074,16 @@
       <c r="E18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="H18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
@@ -845,16 +1094,19 @@
       <c r="E19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="H19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -862,16 +1114,19 @@
       <c r="E20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="H20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <v>100000</v>
@@ -879,16 +1134,19 @@
       <c r="E21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="H21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -896,16 +1154,19 @@
       <c r="E22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="H22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D23">
         <v>100000</v>
@@ -913,16 +1174,19 @@
       <c r="E23" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="H23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -930,16 +1194,19 @@
       <c r="E24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="H24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D25">
         <v>100000</v>
@@ -947,16 +1214,19 @@
       <c r="E25" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="H25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -964,16 +1234,19 @@
       <c r="E26" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="H26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -981,22 +1254,568 @@
       <c r="E27" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="H27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D28">
-        <v>123456</v>
+        <v>0</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
+      </c>
+      <c r="H28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1014,13 +1833,13 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1047,25 +1866,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -1092,25 +1911,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -1137,25 +1956,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -1182,19 +2001,19 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -1221,22 +2040,22 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -1263,25 +2082,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -1302,31 +2121,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
agregado indicadores de valvulas y compuertas
</commit_message>
<xml_diff>
--- a/SCADA/RemoteRuntime/tagsDeAplicacion.xlsx
+++ b/SCADA/RemoteRuntime/tagsDeAplicacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="23655" windowHeight="13035"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="10455" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Registered Tag List" sheetId="9" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="125">
   <si>
     <t>Network Info</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>activa o desactiva el boton de AUTOMATICO en L21</t>
+  </si>
+  <si>
+    <t>l21BtnLiberarAutManEnabled</t>
+  </si>
+  <si>
+    <t>activa o desactiva el boton de LIBERAR AUTO/MAN</t>
   </si>
   <si>
     <t>l21BtnInicioEnabled</t>
@@ -722,16 +728,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -1249,7 +1250,7 @@
         <v>10</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
@@ -1269,7 +1270,7 @@
         <v>10</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -1309,7 +1310,7 @@
         <v>10</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
         <v>11</v>
@@ -1329,7 +1330,7 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
@@ -1429,7 +1430,7 @@
         <v>13</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
@@ -1449,7 +1450,7 @@
         <v>13</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="s">
         <v>11</v>
@@ -1469,7 +1470,7 @@
         <v>13</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="s">
         <v>11</v>
@@ -1489,7 +1490,7 @@
         <v>13</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
         <v>11</v>
@@ -1686,7 +1687,7 @@
         <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -1706,10 +1707,10 @@
         <v>102</v>
       </c>
       <c r="C50" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
         <v>11</v>
@@ -1726,7 +1727,7 @@
         <v>104</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1746,10 +1747,10 @@
         <v>106</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52" t="s">
         <v>11</v>
@@ -1775,7 +1776,7 @@
         <v>11</v>
       </c>
       <c r="H53" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1783,19 +1784,19 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" t="s">
         <v>109</v>
-      </c>
-      <c r="C54" t="s">
-        <v>42</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54" t="s">
-        <v>11</v>
-      </c>
-      <c r="H54" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1806,16 +1807,36 @@
         <v>111</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>13213</v>
       </c>
       <c r="E55" t="s">
         <v>11</v>
       </c>
       <c r="H55" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1833,13 +1854,13 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1866,25 +1887,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -1911,25 +1932,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -1956,25 +1977,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -2001,19 +2022,19 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -2040,22 +2061,22 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -2082,25 +2103,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -2127,25 +2148,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
agregado scada segundo reposo
</commit_message>
<xml_diff>
--- a/SCADA/RemoteRuntime/tagsDeAplicacion.xlsx
+++ b/SCADA/RemoteRuntime/tagsDeAplicacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="10455" windowHeight="5385"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="10455" windowHeight="5385" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Registered Tag List" sheetId="9" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="153">
   <si>
     <t>Network Info</t>
   </si>
@@ -48,6 +48,51 @@
     <t>Information</t>
   </si>
   <si>
+    <t>Profinet / 1</t>
+  </si>
+  <si>
+    <t>CT1_START</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Not Historical</t>
+  </si>
+  <si>
+    <t>CT1_STOP</t>
+  </si>
+  <si>
+    <t>CT1_CONF_START</t>
+  </si>
+  <si>
+    <t>CT1_CONF_STOP</t>
+  </si>
+  <si>
+    <t>CT2_START</t>
+  </si>
+  <si>
+    <t>CT2_STOP</t>
+  </si>
+  <si>
+    <t>CT2_CONF_START</t>
+  </si>
+  <si>
+    <t>CT2_CONF_STOP</t>
+  </si>
+  <si>
+    <t>CT3_START</t>
+  </si>
+  <si>
+    <t>CT3_STOP</t>
+  </si>
+  <si>
+    <t>CT3_CONF_START</t>
+  </si>
+  <si>
+    <t>CT3_CONF_STOP</t>
+  </si>
+  <si>
     <t>Internal</t>
   </si>
   <si>
@@ -57,15 +102,9 @@
     <t>Usigned int16</t>
   </si>
   <si>
-    <t>Not Historical</t>
-  </si>
-  <si>
     <t>l21SourceSelected</t>
   </si>
   <si>
-    <t>Boolean</t>
-  </si>
-  <si>
     <t>l21CmbxSourceEnabled</t>
   </si>
   <si>
@@ -397,6 +436,51 @@
   </si>
   <si>
     <t>Register Table</t>
+  </si>
+  <si>
+    <t>S7300-CPU315-32-PN/DP,192.168.1.80,102,100,0,5000</t>
+  </si>
+  <si>
+    <t>Group 1</t>
+  </si>
+  <si>
+    <t>Cycle 1</t>
+  </si>
+  <si>
+    <t>M 0.0</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>M 0.1</t>
+  </si>
+  <si>
+    <t>M 0.2</t>
+  </si>
+  <si>
+    <t>M 0.3</t>
+  </si>
+  <si>
+    <t>M 0.4</t>
+  </si>
+  <si>
+    <t>M 0.5</t>
+  </si>
+  <si>
+    <t>M 0.6</t>
+  </si>
+  <si>
+    <t>M 0.7</t>
+  </si>
+  <si>
+    <t>M 1.1</t>
+  </si>
+  <si>
+    <t>M 1.2</t>
+  </si>
+  <si>
+    <t>M 1.3</t>
   </si>
 </sst>
 </file>
@@ -728,9 +812,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
@@ -785,7 +869,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -799,10 +883,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -816,7 +900,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -833,10 +917,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -850,10 +934,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -867,10 +951,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -884,7 +968,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -894,9 +978,6 @@
       </c>
       <c r="E9" t="s">
         <v>11</v>
-      </c>
-      <c r="H9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -904,19 +985,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -924,19 +1002,16 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -944,19 +1019,16 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
-      </c>
-      <c r="H12" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -964,7 +1036,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -974,340 +1046,316 @@
       </c>
       <c r="E13" t="s">
         <v>11</v>
-      </c>
-      <c r="H13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
-      </c>
-      <c r="H15" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
-      </c>
-      <c r="H16" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
-      </c>
-      <c r="H17" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
-      </c>
-      <c r="H18" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
-      </c>
-      <c r="H19" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
-      </c>
-      <c r="H20" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D21">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
       </c>
       <c r="H21" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
       </c>
       <c r="H22" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23">
         <v>8</v>
       </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23">
-        <v>100000</v>
-      </c>
       <c r="E23" t="s">
         <v>11</v>
       </c>
       <c r="H23" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
       </c>
       <c r="H24" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D25">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="E25" t="s">
         <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
       </c>
       <c r="H26" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D27">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
       </c>
       <c r="H27" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
       </c>
       <c r="H28" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
       </c>
       <c r="H29" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D30">
         <v>10</v>
@@ -1316,78 +1364,78 @@
         <v>11</v>
       </c>
       <c r="H30" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
       </c>
       <c r="H31" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E32" t="s">
         <v>11</v>
       </c>
       <c r="H32" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>100000</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
       </c>
       <c r="H33" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1396,138 +1444,138 @@
         <v>11</v>
       </c>
       <c r="H34" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="E35" t="s">
         <v>11</v>
       </c>
       <c r="H35" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
       </c>
       <c r="H36" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="E37" t="s">
         <v>11</v>
       </c>
       <c r="H37" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" t="s">
         <v>11</v>
       </c>
       <c r="H38" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E39" t="s">
         <v>11</v>
       </c>
       <c r="H39" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E40" t="s">
         <v>11</v>
       </c>
       <c r="H40" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1536,98 +1584,98 @@
         <v>11</v>
       </c>
       <c r="H41" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E42" t="s">
         <v>11</v>
       </c>
       <c r="H42" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E43" t="s">
         <v>11</v>
       </c>
       <c r="H43" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E44" t="s">
         <v>11</v>
       </c>
       <c r="H44" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E45" t="s">
         <v>11</v>
       </c>
       <c r="H45" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -1636,18 +1684,18 @@
         <v>11</v>
       </c>
       <c r="H46" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1656,78 +1704,78 @@
         <v>11</v>
       </c>
       <c r="H47" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" t="s">
         <v>11</v>
       </c>
       <c r="H48" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B49" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C49" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" t="s">
         <v>11</v>
       </c>
       <c r="H49" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C50" t="s">
         <v>10</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50" t="s">
         <v>11</v>
       </c>
       <c r="H50" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C51" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1736,15 +1784,15 @@
         <v>11</v>
       </c>
       <c r="H51" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
         <v>10</v>
@@ -1756,18 +1804,18 @@
         <v>11</v>
       </c>
       <c r="H52" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -1776,18 +1824,18 @@
         <v>11</v>
       </c>
       <c r="H53" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -1796,47 +1844,287 @@
         <v>11</v>
       </c>
       <c r="H54" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="D55">
-        <v>13213</v>
+        <v>0</v>
       </c>
       <c r="E55" t="s">
         <v>11</v>
       </c>
       <c r="H55" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B56" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+      <c r="H60" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" t="s">
         <v>113</v>
       </c>
-      <c r="C56" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56" t="s">
-        <v>11</v>
-      </c>
-      <c r="H56" t="s">
+      <c r="C61" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>11</v>
+      </c>
+      <c r="H62" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>11</v>
+      </c>
+      <c r="H65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" t="s">
+        <v>123</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>11</v>
+      </c>
+      <c r="H66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" t="s">
+        <v>124</v>
+      </c>
+      <c r="C67" t="s">
+        <v>55</v>
+      </c>
+      <c r="D67">
+        <v>13213</v>
+      </c>
+      <c r="E67" t="s">
+        <v>11</v>
+      </c>
+      <c r="H67" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" t="s">
+        <v>126</v>
+      </c>
+      <c r="C68" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>11</v>
+      </c>
+      <c r="H68" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1854,13 +2142,13 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1887,25 +2175,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -1932,25 +2220,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -1977,25 +2265,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -2022,19 +2310,19 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="E1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -2053,30 +2341,36 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="E1" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -2086,6 +2380,292 @@
       </c>
       <c r="I1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12" t="s">
+        <v>152</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2103,25 +2683,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -2148,25 +2728,25 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>

</xml_diff>